<commit_message>
switched to tree based hashmap to begin calculating lrRatios
</commit_message>
<xml_diff>
--- a/pmf_calcs.xlsx
+++ b/pmf_calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/slogue/IdeaProjects/stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1F42CA-E118-DB46-9BF1-85F2272235BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A331D86-ED53-2349-B549-AE2A9240CACF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{596306AF-DF0F-1E43-B94E-B553941CDB57}"/>
   </bookViews>
@@ -38,9 +38,6 @@
     <t>Particle Size (micrometer)</t>
   </si>
   <si>
-    <t>Bin Heights (%)</t>
-  </si>
-  <si>
     <t>Probability Mass Function</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>Check that all probabilities sum to 1.0:</t>
+  </si>
+  <si>
+    <t>Bin Heights (percent)</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -513,7 +513,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="B4" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -544,20 +544,20 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="L8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="B9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9" s="1">
         <f>(E4/100)</f>
@@ -621,7 +621,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12">
         <f>SUM(E9)/SUM(F9:J9)</f>
@@ -650,17 +650,17 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="7" customFormat="1">
       <c r="A16" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -671,74 +671,74 @@
     </row>
     <row r="20" spans="1:8">
       <c r="C20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E20" s="4">
         <f>SUM(E10*E9, F10*F9, G10*G9, H10*H9, I10*I9, J10*J9)</f>
         <v>14.8</v>
       </c>
       <c r="F20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="C21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="C22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="C23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E23" s="4">
         <f>SUM( E10*E10*E9, F10*F10*F9, G10*G10*G9, H10*H10*H9, I10*I10*I9, J10*J10*J9 ) - (E20*E20)</f>
         <v>34.45999999999998</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="C24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E24" s="5">
         <f>SQRT(E23)</f>
         <v>5.8702640485756667</v>
       </c>
       <c r="F24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="C25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E25" s="5">
         <f>(E24/E20)*100</f>
         <v>39.663946274159905</v>
       </c>
       <c r="F25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>